<commit_message>
data 2014 to 2017
</commit_message>
<xml_diff>
--- a/data/raw_data/mapping_columns.xlsx
+++ b/data/raw_data/mapping_columns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NeueFische\ds-bootcamp-capstone-project\data\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\ds-bootcamp-capstone-project\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{217CB8FA-1D3F-4CC9-8654-403B684A591D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F8FEB4-8CD5-46DE-AF7A-7456375AD74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F033A974-E577-4783-B4F8-C93441CA2000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F033A974-E577-4783-B4F8-C93441CA2000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_columns" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +547,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -710,52 +716,53 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -771,7 +778,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1089,17 +1096,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678A6564-1535-4DB4-B7A8-56EAB03DBDDB}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1123,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1131,7 +1138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1171,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1187,7 +1194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1203,7 +1210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1227,15 +1234,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1243,15 +1250,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1259,7 +1266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1267,7 +1274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1283,7 +1290,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1299,7 +1306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1315,7 +1322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1323,7 +1330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1347,7 +1354,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1363,7 +1370,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1371,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1379,7 +1386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1395,7 +1402,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1411,7 +1418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1419,7 +1426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1427,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1435,7 +1442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -1443,7 +1450,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -1459,7 +1466,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -1467,7 +1474,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -1475,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -1515,7 +1522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1531,7 +1538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -1539,7 +1546,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -1547,7 +1554,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>

</xml_diff>